<commit_message>
Add generate report function
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="5" name="Daily Report" state="show" r:id="rId4"/>
+    <sheet sheetId="4" name="Booking Details" state="show" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -26,19 +27,73 @@
   </si>
   <si>
     <t>No. Not Admitted</t>
+  </si>
+  <si>
+    <t>booking_id</t>
+  </si>
+  <si>
+    <t>session_date</t>
+  </si>
+  <si>
+    <t>session_start</t>
+  </si>
+  <si>
+    <t>session_end</t>
+  </si>
+  <si>
+    <t>station_name</t>
+  </si>
+  <si>
+    <t>role_name</t>
+  </si>
+  <si>
+    <t>14:40:00</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>Aviation Academy</t>
+  </si>
+  <si>
+    <t>Pilot</t>
+  </si>
+  <si>
+    <t>14:20:00</t>
+  </si>
+  <si>
+    <t>15:40:00</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>13:20:00</t>
+  </si>
+  <si>
+    <t>13:40:00</t>
+  </si>
+  <si>
+    <t>Cabin Crew</t>
+  </si>
+  <si>
+    <t>14:00:00</t>
+  </si>
+  <si>
+    <t>15:20:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -342,19 +397,532 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -372,28 +940,20 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A2" s="1">
+        <v>43318.66666666667</v>
+      </c>
+      <c r="B2">
+        <v>160</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>